<commit_message>
feat: update thermal discomfort variable and enhance climate classification links
</commit_message>
<xml_diff>
--- a/backend/data/climatologias_TD.xlsx
+++ b/backend/data/climatologias_TD.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="tdi" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="utci26" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="utci32" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="tdi24" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="tdi28" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="utci26" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="utci32" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="18">
   <si>
     <t xml:space="preserve">Historical</t>
   </si>
@@ -117,7 +118,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -176,9 +177,37 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
       <right/>
       <top style="medium"/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="medium"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -193,27 +222,6 @@
       <right style="medium"/>
       <top style="medium"/>
       <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -242,7 +250,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -291,7 +299,39 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -299,15 +339,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -327,15 +367,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -530,7 +570,7 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -915,7 +955,387 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="12"/>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="16" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="E8" s="16" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="F8" s="16" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="G8" s="4" t="n">
+        <v>0.56</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>2.09</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>2.84</v>
+      </c>
+      <c r="E9" s="16" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="F9" s="16" t="n">
+        <v>4.21</v>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>4.21</v>
+      </c>
+      <c r="H9" s="5" t="n">
+        <v>8.44</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>2.34</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>2.91</v>
+      </c>
+      <c r="E10" s="16" t="n">
+        <v>3.35</v>
+      </c>
+      <c r="F10" s="16" t="n">
+        <v>5.35</v>
+      </c>
+      <c r="G10" s="4" t="n">
+        <v>4.89</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>9.19</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>3.03</v>
+      </c>
+      <c r="E11" s="16" t="n">
+        <v>2.59</v>
+      </c>
+      <c r="F11" s="16" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="G11" s="4" t="n">
+        <v>2.58</v>
+      </c>
+      <c r="H11" s="5" t="n">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="4" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="E12" s="16" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="F12" s="16" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="G12" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H12" s="5" t="n">
+        <v>2.31</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="E13" s="16" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F13" s="16" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G13" s="4" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="18" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -927,7 +1347,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12"/>
+      <c r="A1" s="20"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -945,29 +1365,29 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13"/>
+      <c r="A2" s="21"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="23" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="24" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="6" t="n">
@@ -976,7 +1396,7 @@
       <c r="C3" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="17" t="n">
+      <c r="D3" s="25" t="n">
         <v>0</v>
       </c>
       <c r="E3" s="7" t="n">
@@ -985,7 +1405,7 @@
       <c r="F3" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="17" t="n">
+      <c r="G3" s="25" t="n">
         <v>0</v>
       </c>
       <c r="H3" s="8" t="n">
@@ -993,7 +1413,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="26" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="6" t="n">
@@ -1002,7 +1422,7 @@
       <c r="C4" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="17" t="n">
+      <c r="D4" s="25" t="n">
         <v>0</v>
       </c>
       <c r="E4" s="7" t="n">
@@ -1011,7 +1431,7 @@
       <c r="F4" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="17" t="n">
+      <c r="G4" s="25" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="8" t="n">
@@ -1019,7 +1439,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="26" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="6" t="n">
@@ -1028,7 +1448,7 @@
       <c r="C5" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="17" t="n">
+      <c r="D5" s="25" t="n">
         <v>0</v>
       </c>
       <c r="E5" s="7" t="n">
@@ -1037,7 +1457,7 @@
       <c r="F5" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="17" t="n">
+      <c r="G5" s="25" t="n">
         <v>0</v>
       </c>
       <c r="H5" s="8" t="n">
@@ -1045,7 +1465,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="6" t="n">
@@ -1054,7 +1474,7 @@
       <c r="C6" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="D6" s="17" t="n">
+      <c r="D6" s="25" t="n">
         <v>8.33333333333333E-005</v>
       </c>
       <c r="E6" s="7" t="n">
@@ -1063,7 +1483,7 @@
       <c r="F6" s="8" t="n">
         <v>2.38095238095238E-005</v>
       </c>
-      <c r="G6" s="17" t="n">
+      <c r="G6" s="25" t="n">
         <v>0</v>
       </c>
       <c r="H6" s="8" t="n">
@@ -1071,7 +1491,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="26" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="6" t="n">
@@ -1080,7 +1500,7 @@
       <c r="C7" s="7" t="n">
         <v>0.0526666666666664</v>
       </c>
-      <c r="D7" s="17" t="n">
+      <c r="D7" s="25" t="n">
         <v>0.061327380952381</v>
       </c>
       <c r="E7" s="7" t="n">
@@ -1089,7 +1509,7 @@
       <c r="F7" s="8" t="n">
         <v>0.263446428571428</v>
       </c>
-      <c r="G7" s="17" t="n">
+      <c r="G7" s="25" t="n">
         <v>0.0831488095238098</v>
       </c>
       <c r="H7" s="8" t="n">
@@ -1097,7 +1517,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="26" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="6" t="n">
@@ -1106,7 +1526,7 @@
       <c r="C8" s="7" t="n">
         <v>1.70638095238095</v>
       </c>
-      <c r="D8" s="17" t="n">
+      <c r="D8" s="25" t="n">
         <v>2.05808928571429</v>
       </c>
       <c r="E8" s="7" t="n">
@@ -1115,7 +1535,7 @@
       <c r="F8" s="8" t="n">
         <v>2.26554761904762</v>
       </c>
-      <c r="G8" s="17" t="n">
+      <c r="G8" s="25" t="n">
         <v>1.59374404761905</v>
       </c>
       <c r="H8" s="8" t="n">
@@ -1123,7 +1543,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="26" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="6" t="n">
@@ -1132,7 +1552,7 @@
       <c r="C9" s="7" t="n">
         <v>5.1091726190476</v>
       </c>
-      <c r="D9" s="17" t="n">
+      <c r="D9" s="25" t="n">
         <v>4.81472619047619</v>
       </c>
       <c r="E9" s="7" t="n">
@@ -1141,7 +1561,7 @@
       <c r="F9" s="8" t="n">
         <v>6.81969642857143</v>
       </c>
-      <c r="G9" s="17" t="n">
+      <c r="G9" s="25" t="n">
         <v>6.02869047619048</v>
       </c>
       <c r="H9" s="8" t="n">
@@ -1149,7 +1569,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="26" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="6" t="n">
@@ -1158,7 +1578,7 @@
       <c r="C10" s="7" t="n">
         <v>4.24272619047619</v>
       </c>
-      <c r="D10" s="17" t="n">
+      <c r="D10" s="25" t="n">
         <v>4.85792261904762</v>
       </c>
       <c r="E10" s="7" t="n">
@@ -1167,7 +1587,7 @@
       <c r="F10" s="8" t="n">
         <v>7.03758333333333</v>
       </c>
-      <c r="G10" s="17" t="n">
+      <c r="G10" s="25" t="n">
         <v>6.13823809523808</v>
       </c>
       <c r="H10" s="8" t="n">
@@ -1175,7 +1595,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="26" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="6" t="n">
@@ -1184,7 +1604,7 @@
       <c r="C11" s="7" t="n">
         <v>1.09889285714286</v>
       </c>
-      <c r="D11" s="17" t="n">
+      <c r="D11" s="25" t="n">
         <v>2.12066071428572</v>
       </c>
       <c r="E11" s="7" t="n">
@@ -1193,7 +1613,7 @@
       <c r="F11" s="8" t="n">
         <v>2.86065476190477</v>
       </c>
-      <c r="G11" s="17" t="n">
+      <c r="G11" s="25" t="n">
         <v>1.69494642857143</v>
       </c>
       <c r="H11" s="8" t="n">
@@ -1201,7 +1621,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="6" t="n">
@@ -1210,7 +1630,7 @@
       <c r="C12" s="7" t="n">
         <v>0.00234523809523809</v>
       </c>
-      <c r="D12" s="17" t="n">
+      <c r="D12" s="25" t="n">
         <v>0.017702380952381</v>
       </c>
       <c r="E12" s="7" t="n">
@@ -1219,7 +1639,7 @@
       <c r="F12" s="8" t="n">
         <v>0.00776190476190477</v>
       </c>
-      <c r="G12" s="17" t="n">
+      <c r="G12" s="25" t="n">
         <v>0.00284523809523809</v>
       </c>
       <c r="H12" s="8" t="n">
@@ -1227,7 +1647,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="26" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="6" t="n">
@@ -1236,7 +1656,7 @@
       <c r="C13" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="D13" s="17" t="n">
+      <c r="D13" s="25" t="n">
         <v>0</v>
       </c>
       <c r="E13" s="7" t="n">
@@ -1245,7 +1665,7 @@
       <c r="F13" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="G13" s="17" t="n">
+      <c r="G13" s="25" t="n">
         <v>0</v>
       </c>
       <c r="H13" s="8" t="n">
@@ -1253,7 +1673,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="27" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="9" t="n">
@@ -1262,7 +1682,7 @@
       <c r="C14" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="D14" s="20" t="n">
+      <c r="D14" s="28" t="n">
         <v>0</v>
       </c>
       <c r="E14" s="10" t="n">
@@ -1271,7 +1691,7 @@
       <c r="F14" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="G14" s="20" t="n">
+      <c r="G14" s="28" t="n">
         <v>0</v>
       </c>
       <c r="H14" s="11" t="n">
@@ -1295,14 +1715,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I72" activeCellId="0" sqref="I72"/>
     </sheetView>
   </sheetViews>
@@ -1331,30 +1751,30 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2"/>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="23" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="21" t="n">
+      <c r="B3" s="29" t="n">
         <v>0</v>
       </c>
       <c r="C3" s="7" t="n">
@@ -1363,10 +1783,10 @@
       <c r="D3" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="23" t="n">
+      <c r="E3" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="31" t="n">
         <v>0</v>
       </c>
       <c r="G3" s="7" t="n">
@@ -1377,7 +1797,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="26" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="6" t="n">
@@ -1403,7 +1823,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="26" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="6" t="n">
@@ -1429,7 +1849,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="6" t="n">
@@ -1455,7 +1875,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="26" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="6" t="n">
@@ -1481,7 +1901,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="26" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="6" t="n">
@@ -1507,7 +1927,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="26" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="6" t="n">
@@ -1533,7 +1953,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="26" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="6" t="n">
@@ -1559,7 +1979,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="26" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="6" t="n">
@@ -1585,7 +2005,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="6" t="n">
@@ -1611,7 +2031,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="26" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="6" t="n">
@@ -1637,7 +2057,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="27" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="9" t="n">

</xml_diff>